<commit_message>
updated api project from nishit
</commit_message>
<xml_diff>
--- a/roostifyapitest/test-configuration.xlsx
+++ b/roostifyapitest/test-configuration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="28">
   <si>
     <t>Test Suite</t>
   </si>
@@ -106,7 +106,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="0"/>
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +115,176 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +301,21 @@
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightDown">
+        <bgColor indexed="10"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -145,13 +329,69 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,8 +694,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -532,14 +772,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="1.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="41.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="32.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="4.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="1.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="59.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="41.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="32.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="4.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.90625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -582,7 +822,7 @@
         <v>23</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="61" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -603,7 +843,7 @@
         <v>22</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="59" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -624,7 +864,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="57" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="2" t="s">

</xml_diff>